<commit_message>
Modify all exported files to reflect PCB changes
</commit_message>
<xml_diff>
--- a/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
+++ b/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\2.3B\SinESC-Multi-2.3B\Exported Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\SinESC-Multi\Exported Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119782DA-52E5-4A5B-A3B5-40AEF1217737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FD770D-24E7-4D34-B297-73661869D2F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
     <t>BOM Consolidation Ratio (Total/Unique): 3.261</t>
   </si>
   <si>
-    <t>SinESC Multi v2.3B - Bill of Materials (BOM)</t>
+    <t>SinESC Multi v2.3C - Bill of Materials (BOM)</t>
   </si>
 </sst>
 </file>
@@ -1108,22 +1108,22 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.61328125" customWidth="1"/>
-    <col min="2" max="2" width="63.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.61328125" customWidth="1"/>
-    <col min="4" max="4" width="8.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.84375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.61328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" customWidth="1"/>
+    <col min="2" max="2" width="63.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6328125" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>57</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>58</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>59</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>75</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>73</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>76</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>8</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D11">
         <v>9</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D12">
         <v>10</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D13">
         <v>11</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D14">
         <v>12</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D15">
         <v>13</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D16">
         <v>14</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D17">
         <v>15</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D18">
         <v>16</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D19">
         <v>17</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D20">
         <v>18</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D21">
         <v>19</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D22">
         <v>20</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D23">
         <v>21</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D24">
         <v>22</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D25">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Update "Source" field in BOM to reflect latest file name and path
</commit_message>
<xml_diff>
--- a/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
+++ b/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\SinESC-Multi\Exported Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FD770D-24E7-4D34-B297-73661869D2F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A1C934-2CDD-48A8-9702-881CCFFEA7E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="3850" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>U2, U3, U5</t>
   </si>
   <si>
-    <t>Source: SinESC\Multi Edition\2.3B\SinESC-Multi-2.3B\SinESC-Multi-2.3B.sch</t>
-  </si>
-  <si>
     <t>Generated on: 9/3/2020</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>SinESC Multi v2.3C - Bill of Materials (BOM)</t>
+  </si>
+  <si>
+    <t>Source: SinESC\Multi Edition\SinESC-Multi\SinESC-Multi.sch</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1108,7 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,10 +1125,10 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5">
@@ -1198,7 +1198,7 @@
         <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1218,7 +1218,7 @@
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1295,7 +1295,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -1329,7 +1329,7 @@
         <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -1346,7 +1346,7 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
         <v>22</v>
@@ -1363,7 +1363,7 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
@@ -1380,7 +1380,7 @@
         <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
         <v>24</v>
@@ -1397,7 +1397,7 @@
         <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
@@ -1414,7 +1414,7 @@
         <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
@@ -1431,7 +1431,7 @@
         <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
         <v>27</v>
@@ -1448,7 +1448,7 @@
         <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
         <v>28</v>
@@ -1465,7 +1465,7 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
         <v>30</v>
@@ -1553,7 +1553,7 @@
         <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix another issue in which the bootstrap capacitors were not connected to the source pins of the high-side FETs
</commit_message>
<xml_diff>
--- a/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
+++ b/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\SinESC-Multi\Exported Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A1C934-2CDD-48A8-9702-881CCFFEA7E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5E4BBC-DBD1-4407-9AA3-A75205786C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="3850" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>C1608X5R1E106M080AC</t>
   </si>
   <si>
-    <t>C21</t>
-  </si>
-  <si>
     <t>22nF</t>
   </si>
   <si>
@@ -158,18 +155,6 @@
     <t>8MHz</t>
   </si>
   <si>
-    <t>C1, C2, C4, C8, C17, C20, C30</t>
-  </si>
-  <si>
-    <t>C3, C5, C6, C7, C9, C10, C12, C14, C15, C16</t>
-  </si>
-  <si>
-    <t>C11, C18, C19, C23, C24, C25, C26, C28, C29, C31, C32, C33</t>
-  </si>
-  <si>
-    <t>C13, C22, C34, C35</t>
-  </si>
-  <si>
     <t>Q1, Q2, Q3, Q4, Q5, Q6</t>
   </si>
   <si>
@@ -200,9 +185,6 @@
     <t>U2, U3, U5</t>
   </si>
   <si>
-    <t>Generated on: 9/3/2020</t>
-  </si>
-  <si>
     <t>Tool: Eeschema (5.1.6)-1</t>
   </si>
   <si>
@@ -264,6 +246,24 @@
   </si>
   <si>
     <t>Source: SinESC\Multi Edition\SinESC-Multi\SinESC-Multi.sch</t>
+  </si>
+  <si>
+    <t>C1, C2, C4, C8, C20, C23, C30</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C7, C9, C10, C12, C14, C15, C19</t>
+  </si>
+  <si>
+    <t>C11, C16, C17, C18, C21, C22, C26, C28, C29, C31, C32, C33</t>
+  </si>
+  <si>
+    <t>C13, C25, C34, C35</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>Generated on: 12/30/2020</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1108,7 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,10 +1125,10 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1154,7 +1154,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1174,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5">
@@ -1195,10 +1195,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1215,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1235,18 +1235,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1255,18 +1255,18 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1275,13 +1275,13 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
@@ -1292,13 +1292,13 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
         <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
@@ -1309,13 +1309,13 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
         <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
@@ -1326,13 +1326,13 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
@@ -1343,13 +1343,13 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
@@ -1360,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
@@ -1377,13 +1377,13 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
@@ -1394,13 +1394,13 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.35">
@@ -1411,13 +1411,13 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.35">
@@ -1428,13 +1428,13 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.35">
@@ -1445,13 +1445,13 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.35">
@@ -1462,13 +1462,13 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s">
         <v>29</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.35">
@@ -1479,13 +1479,13 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.35">
@@ -1496,13 +1496,13 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
         <v>33</v>
-      </c>
-      <c r="H22" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.35">
@@ -1513,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
         <v>35</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.35">
@@ -1530,13 +1530,13 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
         <v>38</v>
       </c>
-      <c r="G24" t="s">
-        <v>39</v>
-      </c>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.35">
@@ -1547,13 +1547,13 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" t="s">
         <v>40</v>
       </c>
-      <c r="G25" t="s">
-        <v>41</v>
-      </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add packages/footprints to BOM
</commit_message>
<xml_diff>
--- a/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
+++ b/Multi Edition/SinESC-Multi/Exported Files/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\SinESC-Multi\Exported Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erksampat/Documents/SinESC/Multi Edition/SinESC-Multi/Exported Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5E4BBC-DBD1-4407-9AA3-A75205786C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2EDFAA-0E59-A344-A6F5-016CBF73E01E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Qty</t>
   </si>
@@ -239,12 +237,6 @@
     <t>Total Component Count: 75</t>
   </si>
   <si>
-    <t>BOM Consolidation Ratio (Total/Unique): 3.261</t>
-  </si>
-  <si>
-    <t>SinESC Multi v2.3C - Bill of Materials (BOM)</t>
-  </si>
-  <si>
     <t>Source: SinESC\Multi Edition\SinESC-Multi\SinESC-Multi.sch</t>
   </si>
   <si>
@@ -264,6 +256,54 @@
   </si>
   <si>
     <t>Generated on: 12/30/2020</t>
+  </si>
+  <si>
+    <t>SinESC Multi v2.3C—Bill of Materials (BOM)</t>
+  </si>
+  <si>
+    <t>BOM Consolidation Ratio (Total:Unique): 3.261:1</t>
+  </si>
+  <si>
+    <t>Last Updated: 1/18/2021</t>
+  </si>
+  <si>
+    <t>Package/Footprint</t>
+  </si>
+  <si>
+    <t>C0201</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>SOD-523</t>
+  </si>
+  <si>
+    <t>L1210</t>
+  </si>
+  <si>
+    <t>TDSON-8-1</t>
+  </si>
+  <si>
+    <t>R0201</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>LQFP48-7x7mm-P0.5mm</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>QFN37-EP-7x7mm</t>
+  </si>
+  <si>
+    <t>Resonator_SMD_muRata_CSTxExxV-3Pin_3.0x1.1mm</t>
   </si>
 </sst>
 </file>
@@ -747,9 +787,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1105,47 +1146,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" customWidth="1"/>
-    <col min="2" max="2" width="63.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.6328125" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1154,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1162,10 +1207,13 @@
       <c r="H3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1174,7 +1222,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1182,10 +1230,13 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5">
@@ -1195,7 +1246,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>53</v>
@@ -1203,10 +1254,13 @@
       <c r="H5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1215,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
         <v>54</v>
@@ -1223,10 +1277,13 @@
       <c r="H6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1235,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -1243,10 +1300,13 @@
       <c r="H7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1263,10 +1323,13 @@
       <c r="H8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1283,8 +1346,14 @@
       <c r="H9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
       <c r="D10">
         <v>8</v>
       </c>
@@ -1300,8 +1369,11 @@
       <c r="H10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>9</v>
       </c>
@@ -1317,8 +1389,11 @@
       <c r="H11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>10</v>
       </c>
@@ -1334,8 +1409,11 @@
       <c r="H12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>11</v>
       </c>
@@ -1351,8 +1429,11 @@
       <c r="H13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>12</v>
       </c>
@@ -1368,8 +1449,11 @@
       <c r="H14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>13</v>
       </c>
@@ -1385,8 +1469,11 @@
       <c r="H15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>14</v>
       </c>
@@ -1402,8 +1489,11 @@
       <c r="H16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>15</v>
       </c>
@@ -1419,8 +1509,11 @@
       <c r="H17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>16</v>
       </c>
@@ -1436,8 +1529,11 @@
       <c r="H18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>17</v>
       </c>
@@ -1453,8 +1549,11 @@
       <c r="H19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>18</v>
       </c>
@@ -1470,8 +1569,11 @@
       <c r="H20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>19</v>
       </c>
@@ -1487,8 +1589,11 @@
       <c r="H21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>20</v>
       </c>
@@ -1504,8 +1609,11 @@
       <c r="H22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>21</v>
       </c>
@@ -1521,8 +1629,11 @@
       <c r="H23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>22</v>
       </c>
@@ -1538,8 +1649,11 @@
       <c r="H24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>23</v>
       </c>
@@ -1554,6 +1668,9 @@
       </c>
       <c r="H25" t="s">
         <v>67</v>
+      </c>
+      <c r="I25" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>